<commit_message>
Responsibilities updated and created.
</commit_message>
<xml_diff>
--- a/Responsibility/Responsibility.xlsx
+++ b/Responsibility/Responsibility.xlsx
@@ -35,21 +35,6 @@
     <t>Extra</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1) 19 August.
-2) 21 August.
-3) 24 August.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) 31 August.
-2)
-    a) 23 August.
-    b) 26 August.
-    c) 26 August.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Code:
            1) 20 MCQ of Architecture and GK.
            2) Interface for the user:
@@ -65,42 +50,6 @@
 </t>
   </si>
   <si>
-    <t>Code:
-            1) 20 MCQ of Sport and Lab.
-            2) Sign In Interface.
-            3) Sign Up Interface.
-Documentation:
-                                 1) Development Methodology. 
-                                 2) Tools and Technology.
-                                 3) Conceptual Diagram. 
-                                 4) Prototype.
-                                 5) Developed System.</t>
-  </si>
-  <si>
-    <t>i) Code:
-            a) Front End:
-                                       1) 20 MCQ of Science and Math.
-                                       2) Compile all MCQs and pickle them.
-                                       3) Unpickled and Separating the MCQ into Question, Answer and Choice lists.
-                                       4) Supply the MCQ to the Interface.
-                                       5) Check the answer and keep track of the score.
-                                       6)  Leaderboard showing top 10 highest scoring users.
-                                       7)  Sound for correst &amp; incorrect answer and highest score.
-               b) Back End:
-                                        1) Insert data from Sign Up Interface.
-                                       2) Read and assign data after successful Sign In Interface.
-                                       3) Update score of the topic if greater than the score of the database.
-              c) Compiled and Completed the Front End portion.
-              d) Compiled and Completed the Back End portion.
-              e) Compiled and Completed Final Application.
-ii) Documentation: 
-                                 1) Testing.
-                                 2) Version Control.
-iii) Error/Exception Handling.
-iv) Persistent Storage.
-v) Video.</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -113,27 +62,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1) 17 August.
-2)
-    a) 30 August.
-   b) 30 August.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code:
-            1) 20 MCQ of Programming and Politics.
-            2) Database:
-                                     a) Create Database.
-                                    b) Delete the current user data from the database.
-Documentation:
-                                  1) System Architecture. 
-                                  2) Project Plan.
-                                  3) Conclusion.
-                                  4) Reference.
-                                  5) Appendix.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">4) Aditya Bharti.
 </t>
   </si>
@@ -147,10 +75,6 @@
   </si>
   <si>
     <t xml:space="preserve">3) Abhinav Dev Bhatta.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)  Supervising Documentation.
 </t>
   </si>
   <si>
@@ -191,12 +115,121 @@
 </t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1)  Supervising Documentation.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Code:
+            1) 20 MCQ of Programming and Politics.
+            2) Database:
+                                     a) Create Database.
+                                    b) Delete the current user data from the database.
+Documentation:
+                                  1) Conclusion.
+                                  2) Appendix.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i) Code:
+            a) Front End:
+                                       1) 20 MCQ of Science and Math.
+                                       2) Compile all MCQs and pickle them.
+                                       3) Unpickled and Separating the MCQ into Question, Answer and Choice lists.
+                                       4) Supply the MCQ to the Interface.
+                                       5) Check the answer and keep track of the score.
+                                       6)  Leaderboard showing top 10 highest scoring users.
+                                       7)  Sound for correst &amp; incorrect answer and highest score.
+               b) Back End:
+                                        1) Insert data from Sign Up Interface.
+                                       2) Read and assign data after successful Sign In Interface.
+                                       3) Update score of the topic if greater than the score of the database.
+              c) Compiled and Completed the Front End portion.
+              d) Compiled and Completed the Back End portion.
+              e) Compiled and Completed Final Application.
+ii) Documentation: 
+                                  1) Testing.
+                                 2) Version Control.
+                                 3) System Architecture. 
+                                 4) Project Plan.
+iii) Error/Exception Handling.
+iv) Persistent Storage.
+v) Video.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code:
+            1) 20 MCQ of Sport and Lab.
+            2) Sign In Interface.
+            3) Sign Up Interface.
+Documentation:
+                                 1) Development Methodology. 
+                                 2) Tools and Technology.
+                                 3) Conceptual Diagram. 
+                                 4) Prototype.
+                                 5) Developed System.
+                                 6)  Reference.
+                                 7) Compiling and completing whole documentation.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1) 19 August.
+2) 21 August.
+3) 24 August.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 31 August.
+2)
+    a) 23 August.
+    b) 26 August.
+    c) 26 August.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 17 August.
+2)
+    a) 30 August.
+   b) 30 August.
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +272,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -364,13 +411,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -655,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,8 +734,8 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>8</v>
+      <c r="C5" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -696,53 +743,53 @@
     </row>
     <row r="6" spans="1:4" ht="408.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="309" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="315.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="239.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="293.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>4</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="379.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2"/>
     </row>

</xml_diff>

<commit_message>
Stand alone exe file created and Responsibilities updated.
</commit_message>
<xml_diff>
--- a/Responsibility/Responsibility.xlsx
+++ b/Responsibility/Responsibility.xlsx
@@ -161,7 +161,44 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">i) Code:
+    <t xml:space="preserve">Code:
+            1) 20 MCQ of Sport and Lab.
+            2) Sign In Interface.
+            3) Sign Up Interface.
+Documentation:
+                                 1) Development Methodology. 
+                                 2) Tools and Technology.
+                                 3) Conceptual Diagram. 
+                                 4) Prototype.
+                                 5) Developed System.
+                                 6)  Reference.
+                                 7) Compiling and completing whole documentation.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1) 19 August.
+2) 21 August.
+3) 24 August.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 31 August.
+2)
+    a) 23 August.
+    b) 26 August.
+    c) 26 August.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 17 August.
+2)
+    a) 30 August.
+   b) 30 August.
+</t>
+  </si>
+  <si>
+    <t>i) Code:
             a) Front End:
                                        1) 20 MCQ of Science and Math.
                                        2) Compile all MCQs and pickle them.
@@ -185,44 +222,7 @@
 iii) Error/Exception Handling.
 iv) Persistent Storage.
 v) Video.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code:
-            1) 20 MCQ of Sport and Lab.
-            2) Sign In Interface.
-            3) Sign Up Interface.
-Documentation:
-                                 1) Development Methodology. 
-                                 2) Tools and Technology.
-                                 3) Conceptual Diagram. 
-                                 4) Prototype.
-                                 5) Developed System.
-                                 6)  Reference.
-                                 7) Compiling and completing whole documentation.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1) 19 August.
-2) 21 August.
-3) 24 August.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) 31 August.
-2)
-    a) 23 August.
-    b) 26 August.
-    c) 26 August.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) 17 August.
-2)
-    a) 30 August.
-   b) 30 August.
-</t>
+vi) Stand Alone Executable File.</t>
   </si>
 </sst>
 </file>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +746,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>10</v>
@@ -760,10 +760,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>11</v>
@@ -777,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -789,7 +789,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2"/>
     </row>

</xml_diff>